<commit_message>
Updated input data for example run
</commit_message>
<xml_diff>
--- a/input_data/The_Vale.xlsx
+++ b/input_data/The_Vale.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9048" activeTab="5" xr2:uid="{7524E475-62B2-4293-879C-84C34393B30D}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9048" activeTab="6" xr2:uid="{7524E475-62B2-4293-879C-84C34393B30D}"/>
   </bookViews>
   <sheets>
     <sheet name="T" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="14">
   <si>
     <t>Elms</t>
   </si>
@@ -2980,59 +2980,16 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE71DCD0-A8A9-47BB-B8B7-8F3F444C3A5A}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
         <v>11</v>
       </c>
     </row>
@@ -3043,492 +3000,132 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34C11937-FC18-4B70-9E19-B50C5AC5AF25}">
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:A24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1">
-        <v>7654</v>
-      </c>
-      <c r="B1">
-        <v>41.82</v>
-      </c>
-      <c r="C1">
-        <v>3.38</v>
-      </c>
-      <c r="D1">
-        <v>0.25</v>
-      </c>
-      <c r="E1">
-        <v>0.02</v>
-      </c>
-      <c r="F1">
-        <v>81.2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+        <v>7780.67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>7859.75</v>
-      </c>
-      <c r="B2">
-        <v>0.47</v>
-      </c>
-      <c r="C2">
-        <v>0.28999999999999998</v>
-      </c>
-      <c r="D2">
-        <v>37.01</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>8.3800000000000008</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+        <v>7905.9000000000005</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>16351.06</v>
-      </c>
-      <c r="B3">
-        <v>341.62999999999897</v>
-      </c>
-      <c r="C3">
-        <v>24.0899999999999</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>258.82</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+        <v>16975.599999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>1915.96999999999</v>
-      </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4">
-        <v>0.34</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+        <v>1916.3099999999899</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>53.97</v>
-      </c>
-      <c r="B5">
-        <v>16580.199999999899</v>
-      </c>
-      <c r="C5">
-        <v>15.79</v>
-      </c>
-      <c r="D5">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="E5">
-        <v>0.22</v>
-      </c>
-      <c r="F5">
-        <v>124.63</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+        <v>16774.949999999903</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>65.399999999999906</v>
-      </c>
-      <c r="B6">
-        <v>23260.28</v>
-      </c>
-      <c r="C6">
-        <v>0.86</v>
-      </c>
-      <c r="D6">
-        <v>55.65</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <v>45.18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+        <v>23427.370000000003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>653.24</v>
-      </c>
-      <c r="B7">
-        <v>122972.97999999901</v>
-      </c>
-      <c r="C7">
-        <v>227.19</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7">
-        <v>866.53</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+        <v>124719.93999999901</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>0</v>
-      </c>
-      <c r="B8">
-        <v>3429.26999999999</v>
-      </c>
-      <c r="C8">
-        <v>2.12</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+        <v>3431.3899999999899</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>2.99</v>
-      </c>
-      <c r="B9">
-        <v>7.8699999999999903</v>
-      </c>
-      <c r="C9">
-        <v>1986.64</v>
-      </c>
-      <c r="D9">
-        <v>0.08</v>
-      </c>
-      <c r="E9">
-        <v>0.01</v>
-      </c>
-      <c r="F9">
-        <v>3.73</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+        <v>2001.32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>1.36</v>
-      </c>
-      <c r="B10">
-        <v>0</v>
-      </c>
-      <c r="C10">
-        <v>5215.68</v>
-      </c>
-      <c r="D10">
-        <v>4.72</v>
-      </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+        <v>5221.76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>24.25</v>
-      </c>
-      <c r="B11">
-        <v>76.689999999999898</v>
-      </c>
-      <c r="C11">
-        <v>11981.96</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-      <c r="F11">
-        <v>30.83</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+        <v>12113.73</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>0</v>
-      </c>
-      <c r="B12">
-        <v>0.02</v>
-      </c>
-      <c r="C12">
-        <v>118.7</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
-      <c r="F12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+        <v>118.72</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>99.63</v>
-      </c>
-      <c r="B13">
-        <v>55.77</v>
-      </c>
-      <c r="C13">
-        <v>7.22</v>
-      </c>
-      <c r="D13">
-        <v>16710.47</v>
-      </c>
-      <c r="E13">
-        <v>0.25</v>
-      </c>
-      <c r="F13">
-        <v>54.529999999999902</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+        <v>16927.87</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>17.329999999999998</v>
-      </c>
-      <c r="B14">
-        <v>1.79</v>
-      </c>
-      <c r="C14">
-        <v>0.24</v>
-      </c>
-      <c r="D14">
-        <v>10395.52</v>
-      </c>
-      <c r="E14">
-        <v>0</v>
-      </c>
-      <c r="F14">
-        <v>9.0299999999999994</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+        <v>10423.910000000002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>361.19</v>
-      </c>
-      <c r="B15">
-        <v>716.219999999999</v>
-      </c>
-      <c r="C15">
-        <v>38.369999999999997</v>
-      </c>
-      <c r="D15">
-        <v>67637.279999999999</v>
-      </c>
-      <c r="E15">
-        <v>0</v>
-      </c>
-      <c r="F15">
-        <v>225.73</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+        <v>68978.789999999994</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>0</v>
-      </c>
-      <c r="B16">
-        <v>0.12</v>
-      </c>
-      <c r="C16">
-        <v>1.21</v>
-      </c>
-      <c r="D16">
-        <v>10006.969999999999</v>
-      </c>
-      <c r="E16">
-        <v>0</v>
-      </c>
-      <c r="F16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+        <v>10008.299999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17">
-        <v>11.35</v>
-      </c>
-      <c r="B17">
-        <v>37.28</v>
-      </c>
-      <c r="C17">
-        <v>2.88</v>
-      </c>
-      <c r="D17">
-        <v>0.49</v>
-      </c>
-      <c r="E17">
-        <v>10441.14</v>
-      </c>
-      <c r="F17">
-        <v>13.08</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+        <v>10506.22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="B18">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="C18">
-        <v>0.26</v>
-      </c>
-      <c r="D18">
-        <v>133.6</v>
-      </c>
-      <c r="E18">
-        <v>14952.82</v>
-      </c>
-      <c r="F18">
-        <v>0.56000000000000005</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+        <v>15089.679999999998</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19">
-        <v>149.31</v>
-      </c>
-      <c r="B19">
-        <v>681.9</v>
-      </c>
-      <c r="C19">
-        <v>40.56</v>
-      </c>
-      <c r="D19">
-        <v>0</v>
-      </c>
-      <c r="E19">
-        <v>54168.68</v>
-      </c>
-      <c r="F19">
-        <v>145.36000000000001</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+        <v>55185.81</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20">
-        <v>0</v>
-      </c>
-      <c r="B20">
-        <v>0.17</v>
-      </c>
-      <c r="C20">
-        <v>0.21</v>
-      </c>
-      <c r="D20">
-        <v>0</v>
-      </c>
-      <c r="E20">
-        <v>3787.35</v>
-      </c>
-      <c r="F20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+        <v>3787.73</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21">
-        <v>121.679999999999</v>
-      </c>
-      <c r="B21">
-        <v>41.1</v>
-      </c>
-      <c r="C21">
-        <v>6.53</v>
-      </c>
-      <c r="D21">
-        <v>0.67</v>
-      </c>
-      <c r="E21">
-        <v>0.05</v>
-      </c>
-      <c r="F21">
-        <v>7411.23</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+        <v>7581.2599999999984</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22">
-        <v>30.93</v>
-      </c>
-      <c r="B22">
-        <v>1.61</v>
-      </c>
-      <c r="C22">
-        <v>1.39</v>
-      </c>
-      <c r="D22">
-        <v>49.629999999999903</v>
-      </c>
-      <c r="E22">
-        <v>0</v>
-      </c>
-      <c r="F22">
-        <v>10664.5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+        <v>10748.06</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23">
-        <v>327.49</v>
-      </c>
-      <c r="B23">
-        <v>421.07</v>
-      </c>
-      <c r="C23">
-        <v>37.25</v>
-      </c>
-      <c r="D23">
-        <v>0</v>
-      </c>
-      <c r="E23">
-        <v>0</v>
-      </c>
-      <c r="F23">
-        <v>22604.23</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+        <v>23390.04</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24">
-        <v>0</v>
-      </c>
-      <c r="B24">
-        <v>0.37</v>
-      </c>
-      <c r="C24">
-        <v>0.61</v>
-      </c>
-      <c r="D24">
-        <v>0</v>
-      </c>
-      <c r="E24">
-        <v>0</v>
-      </c>
-      <c r="F24">
-        <v>975.79</v>
+        <v>976.77</v>
       </c>
     </row>
   </sheetData>
@@ -3538,10 +3135,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2C1BA34-2055-47DB-B60C-CBEF613013B5}">
-  <dimension ref="A1:B36"/>
+  <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3748,7 +3345,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26">
-        <v>5856.3</v>
+        <v>4398.9199999999901</v>
       </c>
       <c r="B26">
         <v>0</v>
@@ -3756,7 +3353,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27">
-        <v>4398.9199999999901</v>
+        <v>700.93999999999903</v>
       </c>
       <c r="B27">
         <v>0</v>
@@ -3764,7 +3361,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28">
-        <v>36175.699999999997</v>
+        <v>435.14</v>
       </c>
       <c r="B28">
         <v>0</v>
@@ -3772,7 +3369,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29">
-        <v>700.93999999999903</v>
+        <v>4.5399999999999903</v>
       </c>
       <c r="B29">
         <v>0</v>
@@ -3780,7 +3377,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30">
-        <v>5889.67</v>
+        <v>1865.3899999999901</v>
       </c>
       <c r="B30">
         <v>0</v>
@@ -3788,49 +3385,9 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31">
-        <v>435.14</v>
+        <v>98823.909999999989</v>
       </c>
       <c r="B31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A32">
-        <v>24345.57</v>
-      </c>
-      <c r="B32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A33">
-        <v>4.5399999999999903</v>
-      </c>
-      <c r="B33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A34">
-        <v>15110.48</v>
-      </c>
-      <c r="B34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A35">
-        <v>1865.3899999999901</v>
-      </c>
-      <c r="B35">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A36">
-        <v>11446.19</v>
-      </c>
-      <c r="B36">
         <v>0</v>
       </c>
     </row>

</xml_diff>